<commit_message>
yorum tabı eklendi olumlu dönüşler pop up
</commit_message>
<xml_diff>
--- a/Kitap1.xlsx
+++ b/Kitap1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\erden.aydogdu\Desktop\Feedback\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D748A442-4CCE-4368-A3DF-D124B9857CAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CCCEC7B-79EC-4BCD-ABA8-9A9B0CEE6040}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1520" yWindow="1520" windowWidth="19200" windowHeight="11170" xr2:uid="{195D167A-9D10-47B3-B6CD-5EAF818A6979}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="19200" windowHeight="11170" xr2:uid="{195D167A-9D10-47B3-B6CD-5EAF818A6979}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>AD-SOYAD</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Gökhan abi</t>
+  </si>
+  <si>
+    <t>özgeabla</t>
+  </si>
+  <si>
+    <t>0 507 002 31 24</t>
+  </si>
+  <si>
+    <t>0 505 642 04 13</t>
+  </si>
+  <si>
+    <t>mustafaonurgirisken</t>
   </si>
 </sst>
 </file>
@@ -497,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0F8748E-2CEF-450F-BF9F-B6FBE3916AD4}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -576,6 +588,28 @@
         <v>3</v>
       </c>
     </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" s="7" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>